<commit_message>
finished sowballing papers research
</commit_message>
<xml_diff>
--- a/5_Snowballing/Backword_Snowballing_1.xlsx
+++ b/5_Snowballing/Backword_Snowballing_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoniotrovato/Documents/GitHub/RegressionTestingOptimizationSLR/5_Snowballing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673DBE51-EEDA-0342-BC82-917ADD33402A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADFA089-48EE-B34B-89AD-38C3B864CC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22540" yWindow="7500" windowWidth="22280" windowHeight="11800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1739" uniqueCount="1217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="1231">
   <si>
     <t>ID</t>
   </si>
@@ -3729,6 +3729,58 @@
   </si>
   <si>
     <t>Composite services evolve for various reasons. Test case selection in the regression testing is an effective technique to ensure the correctness of modified versions meanwhile to reduce the cost of testing. However, few work has studied the test case selection problem based on the data flow testing criteria. In addition, there are three observable kinds of changes during the evolution, including Process change, Binding change and Interface change, which all bring impact to the data flow. To address these issues, a test case selection approach is proposed for regression testing of BPEL (Business Process Execution Language) composite service where all-uses criterion is satisfied and all the three change types are involved. BPEL composite service is modeled with a two-level model in which XCFG (eXtended Control Flow Graph) describes the behavior of BPEL process in the first level and WSDM (Web Service Description Model) depicts the interface information of composite service and partner services in the second level. Change impact analysis is performed to identify the affected definition-use pairs by comparing and analyzing two-level models of the baseline and evolved versions. And testing paths are generated to cover the affected definition-use pairs and select test cases based on the path condition analysis. Empirical result shows that the proposed approach is effective.</t>
+  </si>
+  <si>
+    <t>An extensive study of static regression test selection in modern software evolution</t>
+  </si>
+  <si>
+    <t>O Legunsen, F Hariri, A Shi, Y Lu, L Zhang, D Marinov</t>
+  </si>
+  <si>
+    <t>Regression test selection (RTS) aims to reduce regression testing time by only re-running the tests affected by code changes. Prior research on RTS can be broadly split into dy namic and static techniques. A recently developed dynamic RTS technique called Ekstazi is gaining some adoption in practice, and its evaluation shows that selecting tests at a coarser, class-level granularity provides better results than selecting tests at a finer, method-level granularity. As dynamic RTS is gaining adoption, it is timely to also evaluate static RTS techniques, some of which were proposed over three decades ago but not extensively evaluated on modern software projects.
+This paper presents the first extensive study that evaluates the performance benefits of static RTS techniques and their safety; a technique is safe if it selects to run all tests that may be affected by code changes. We implemented two static RTS techniques, one class-level and one method-level, and compare several variants of these techniques. We also compare these static RTS techniques against Ekstazi, a state-of-the-art, class-level, dynamic RTS technique. The experimental results on 985 revisions of 22 open-source projects show that the class-level static RTS technique is comparable to Ekstazi, with similar performance benefits, but at the risk of being unsafe sometimes. In contrast, the method-level static RTS technique performs rather poorly.</t>
+  </si>
+  <si>
+    <t>Hybrid regression test selection</t>
+  </si>
+  <si>
+    <t>Proceedings of the 40th International Conference on Software Engineering, 2018</t>
+  </si>
+  <si>
+    <t>L Zhang</t>
+  </si>
+  <si>
+    <t>Regression testing is crucial but can be extremely costly. Regression Test Selection (RTS) aims to reduce regression testing cost by only selecting and running the tests that may be affected by code changes. To date, various RTS techniques analyzing at different granularities (e.g., at the basic-block, method, and file levels) have been proposed. RTS techniques working on finer granularities may be more precise in selecting tests, while techniques working on coarser granularities may have lower overhead. According to a recent study, RTS at the file level (FRTS) can have less overall testing time compared with a finer grained technique at the method level, and represents state-of-the-art RTS. In this paper, we present the first hybrid RTS approach, HyRTS, that analyzes at multiple granularities to combine the strengths of traditional RTS techniques at different granularities. We implemented the basic HyRTS technique by combining the method and file granularity RTS. The experimental results on 2707 revisions of 32 projects, totalling over 124 Million LoC, demonstrate that HyRTS outperforms state-of-the-art FRTS significantly in terms of selected test ratio and the offline testing time. We also studied the impacts of each type of method-level changes, and further designed two new HyRTS variants based on the study results. Our additional experiments show that transforming instance method additions/deletions into file-level changes produces an even more effective HyRTS variant that can significantly outperform FRTS in both offline and online testing time.</t>
+  </si>
+  <si>
+    <t>State of practical applicability of regression testing research: A live systematic literature review</t>
+  </si>
+  <si>
+    <t>R Greca, B Miranda, A Bertolino</t>
+  </si>
+  <si>
+    <t>ACM Computing Surveys, 2023</t>
+  </si>
+  <si>
+    <t>Context
+Software regression testing refers to rerunning test cases after the system under test is modified, ascertaining that the changes have not (re-)introduced failures. Not all researchers’ approaches consider applicability and scalability concerns, and not many have produced an impact in practice.
+Objective
+One goal is to investigate industrial relevance and applicability of proposed approaches. Another is providing a live review, open to continuous updates by the community.
+Method
+A systematic review of regression testing studies that are clearly motivated by or validated against industrial relevance and applicability is conducted. It is complemented by follow-up surveys with authors of the selected papers and 23 practitioners.
+Results
+A set of 79 primary studies published between 2016–2022 is collected and classified according to approaches and metrics. Aspects relative to their relevance and impact are discussed, also based on their authors’ feedback. All the data are made available from the live repository that accompanies the study.
+Conclusions
+While widely motivated by industrial relevance and applicability, not many approaches are evaluated in industrial or large-scale open-source systems, and even fewer approaches have been adopted in practice. Some challenges hindering the implementation of relevant approaches are synthesized, also based on the practitioners’ feedback.</t>
+  </si>
+  <si>
+    <t>Hansie: Hybrid and consensus regression test prioritization</t>
+  </si>
+  <si>
+    <t>Shouvick Mondal, Rupesh Nasre</t>
+  </si>
+  <si>
+    <t>Traditionally, given a test-suite and the underlying system-under-test, existing test-case prioritization heuristics report a permutation of the original test-suite that is seemingly best according to their criteria. However, we observe that a single heuristic does not perform optimally in all possible scenarios, given the diverse nature of software and its changes. Hence, multiple individual heuristics exhibit effectiveness differently. Interestingly, together, the heuristics bear the potential of improving the overall regression test selection across scenarios. In this paper, we pose the test-case prioritization as a rank aggregation problem from social choice theory. Our solution approach, named Hansie, is two-flavored: one involving priority-aware hybridization, and the other involving priority-blind computation of a consensus ordering from individual prioritizations. To speed-up test-execution, Hansie executes the aggregated test-case orderings in a parallel multi-processed manner leveraging regular windows in the absence of ties, and irregular windows in the presence of ties. We show the benefit of test-execution after prioritization and introduce a cost-cognizant metric (EPL) for quantifying overall timeline latency due to load-imbalance arising from uniform or non-uniform parallelization windows. We evaluate Hansie on 20 open-source subjects totaling 287,530 lines of source code, 69,305 test-cases, and with parallelization support of up to 40 logical CPUs.</t>
   </si>
 </sst>
 </file>
@@ -4112,10 +4164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO178"/>
+  <dimension ref="A1:AO182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V84" workbookViewId="0">
-      <selection activeCell="AO100" sqref="AO100"/>
+    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
+      <selection activeCell="F183" sqref="F183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8755,6 +8807,9 @@
       <c r="AN101" t="s">
         <v>952</v>
       </c>
+      <c r="AO101" t="s">
+        <v>1010</v>
+      </c>
     </row>
     <row r="102" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
@@ -8802,6 +8857,9 @@
       <c r="AN102" t="s">
         <v>953</v>
       </c>
+      <c r="AO102" t="s">
+        <v>1010</v>
+      </c>
     </row>
     <row r="103" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
@@ -8849,6 +8907,9 @@
       <c r="AN103" t="s">
         <v>953</v>
       </c>
+      <c r="AO103" t="s">
+        <v>1010</v>
+      </c>
     </row>
     <row r="104" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
@@ -8899,6 +8960,9 @@
       <c r="AN104" t="s">
         <v>953</v>
       </c>
+      <c r="AO104" t="s">
+        <v>1010</v>
+      </c>
     </row>
     <row r="105" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
@@ -8946,6 +9010,9 @@
       <c r="AN105" t="s">
         <v>953</v>
       </c>
+      <c r="AO105" t="s">
+        <v>1010</v>
+      </c>
     </row>
     <row r="106" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
@@ -8993,6 +9060,9 @@
       <c r="AN106" t="s">
         <v>953</v>
       </c>
+      <c r="AO106" t="s">
+        <v>1010</v>
+      </c>
     </row>
     <row r="107" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
@@ -9040,6 +9110,9 @@
       <c r="AN107" t="s">
         <v>953</v>
       </c>
+      <c r="AO107" t="s">
+        <v>1010</v>
+      </c>
     </row>
     <row r="108" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
@@ -9090,6 +9163,9 @@
       <c r="AN108" t="s">
         <v>953</v>
       </c>
+      <c r="AO108" t="s">
+        <v>1010</v>
+      </c>
     </row>
     <row r="109" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
@@ -9137,6 +9213,9 @@
       <c r="AN109" t="s">
         <v>953</v>
       </c>
+      <c r="AO109" t="s">
+        <v>1010</v>
+      </c>
     </row>
     <row r="110" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
@@ -9184,6 +9263,9 @@
       <c r="AN110" t="s">
         <v>953</v>
       </c>
+      <c r="AO110" t="s">
+        <v>1010</v>
+      </c>
     </row>
     <row r="111" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
@@ -10569,6 +10651,86 @@
         <v>1216</v>
       </c>
       <c r="AN178" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="179" spans="3:40" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C179" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D179" t="s">
+        <v>1178</v>
+      </c>
+      <c r="E179" t="s">
+        <v>1217</v>
+      </c>
+      <c r="F179">
+        <v>2016</v>
+      </c>
+      <c r="J179" s="3" t="s">
+        <v>1219</v>
+      </c>
+      <c r="AN179" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="180" spans="3:40" x14ac:dyDescent="0.2">
+      <c r="C180" t="s">
+        <v>1222</v>
+      </c>
+      <c r="D180" t="s">
+        <v>1221</v>
+      </c>
+      <c r="E180" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F180">
+        <v>2018</v>
+      </c>
+      <c r="J180" t="s">
+        <v>1223</v>
+      </c>
+      <c r="AN180" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="181" spans="3:40" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C181" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D181" t="s">
+        <v>1226</v>
+      </c>
+      <c r="E181" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F181">
+        <v>2023</v>
+      </c>
+      <c r="J181" s="3" t="s">
+        <v>1227</v>
+      </c>
+      <c r="AN181" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="182" spans="3:40" x14ac:dyDescent="0.2">
+      <c r="C182" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D182" t="s">
+        <v>823</v>
+      </c>
+      <c r="E182" t="s">
+        <v>1228</v>
+      </c>
+      <c r="F182">
+        <v>2021</v>
+      </c>
+      <c r="J182" t="s">
+        <v>1230</v>
+      </c>
+      <c r="AN182" t="s">
         <v>953</v>
       </c>
     </row>

</xml_diff>